<commit_message>
add subcategory, edit subcategory updated
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -103,19 +103,35 @@
   </si>
   <si>
     <t>TC002_Verifylogin</t>
+  </si>
+  <si>
+    <t>TC004_addSubCategory</t>
+  </si>
+  <si>
+    <t>Acetonicpoly</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF484343"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,11 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,20 +703,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>28</v>
       </c>
@@ -724,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -735,8 +755,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>